<commit_message>
some new data classes
</commit_message>
<xml_diff>
--- a/mylib/Data_sample.xlsx
+++ b/mylib/Data_sample.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,311 +440,77 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>prestigeid</t>
+          <t>UserId</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>daykey</t>
+          <t>JourneyDate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>date_key</t>
+          <t>TransportMode</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>devicekey</t>
+          <t>StartTime</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>routeid</t>
+          <t>EndTime</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>jnystatus</t>
+          <t>StartStation</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mode</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>stationofentrykey</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>nlc</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>exit_station_name</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>end_to_end_jny</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>transactiontime</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
+          <t>EndStation</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>541118557</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>11566</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="C2" s="2" t="n">
         <v>40787</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>TransportEnum.RAIL</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>8008</t>
+          <t>09:42:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>end_time         614
+end_time    10:14:00
+Name: 1, dtype: object</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ENTC</t>
+          <t>Bounds Green</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Bounds Green</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>527</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
           <t>Angel</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Bounds Green Angel</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>582</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>09:42:00</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>10:14:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>541118557</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>11566</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>40787</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7715</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ENTC</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Angel</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>507</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Wood Green</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Angel Wood Green</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>798</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>829</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>13:18:00</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>13:49:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>541118557</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>11566</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>40787</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>221</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>BUS</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>221</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>221</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>221</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>862</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>525</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>14:22:00</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>08:45:00</t>
         </is>
       </c>
     </row>

</xml_diff>